<commit_message>
Result of zdemo_excel15_04 evolved (oddHeader)
The result of zdemo_excel15_04 evolved due to this PR: https://github.com/abap2xlsx/abap2xlsx/pull/1144.
Fix #43.
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_04.w3mi.data.xlsx
+++ b/src/zdemo_excel15_04.w3mi.data.xlsx
@@ -383,6 +383,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.39" footer="0.39"/>
   <pageSetup fitToHeight="0" fitToWidth="2" orientation="landscape" paperSize="9" scale="80"/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -430,6 +431,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -456,6 +458,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -495,6 +498,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Result of zdemo_excel15_04 evolved (oddHeader) (#44)
The result of zdemo_excel15_04 evolved due to this PR: https://github.com/abap2xlsx/abap2xlsx/pull/1144.
Fix #43.
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_04.w3mi.data.xlsx
+++ b/src/zdemo_excel15_04.w3mi.data.xlsx
@@ -383,6 +383,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.39" footer="0.39"/>
   <pageSetup fitToHeight="0" fitToWidth="2" orientation="landscape" paperSize="9" scale="80"/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -430,6 +431,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -456,6 +458,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -495,6 +498,7 @@
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>
   <headerFooter>
+    <oddHeader>&amp;L&amp;"-,Standard"&amp;R&amp;"Arial,Standard"&amp;8print date &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;"-,Standard"&amp;L&amp;"Arial,Standard"&amp;8&amp;Z&amp;F&amp;R&amp;"Arial,Standard"&amp;8page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>